<commit_message>
add williamchong (Liker Land) A1-A6 evidence
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>TeamName</t>
   </si>
@@ -121,12 +121,30 @@
     <t>class id you issued</t>
   </si>
   <si>
+    <t>F9D6A76D97EE94FA4BFBEB7FB9807E14EE19FFEA5909CA83C22B93970131064B</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
     <t>NFTID</t>
   </si>
   <si>
     <t>nft id you minted</t>
   </si>
   <si>
+    <t>73E3720846E6EA59D7B39ADE2122FB2D3CEA698D87E56E7243A06BAB5855BF04</t>
+  </si>
+  <si>
+    <t>like1</t>
+  </si>
+  <si>
+    <t>5B69CC52AD5243DF811A967AFEF4C4CB83327251CA44AC4395F7158FEFA66E4B</t>
+  </si>
+  <si>
+    <t>like2</t>
+  </si>
+  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -139,10 +157,34 @@
     <t>dest chain id</t>
   </si>
   <si>
+    <t>08E95B608EFE04518CCE6FBFD050059BFDE5A99ECE2247C5BF5AC8FC55E48426</t>
+  </si>
+  <si>
+    <t>stars1jt4zg8hdvavvx5ese9cyx2p3yfqzm7h27vjnm097u29zxs8hkg4qc6mmuy</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>C2B9F79318B192C18C97A46B4C2A3C0E757F341136842DD3A9AA66BBFF3540DF</t>
+  </si>
+  <si>
+    <t>ibc/37A82AA36EC33544358288B5DB0F27D108B282792161744EBC866F8F9D231C87</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
     <t>tx hash on dest chain</t>
   </si>
   <si>
     <t>ibc class on chain</t>
+  </si>
+  <si>
+    <t>AB85B3B1363C71657FB62C2BEDEF814EF5C12DE92C097B959C88ACF2F09D8FD3</t>
+  </si>
+  <si>
+    <t>3179F724E31D62F798F6F314DB6FABF158BD017CC49BDF1695BEFCC1F88BE310</t>
   </si>
   <si>
     <t>tx hash on that chain</t>
@@ -194,7 +236,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -337,34 +385,34 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -403,7 +451,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -657,17 +705,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -695,10 +743,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -946,12 +994,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1238,7 +1286,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1266,10 +1314,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1712,7 +1760,7 @@
         <v>25</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -1720,10 +1768,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1812,7 +1860,7 @@
         <v>25</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -1820,10 +1868,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1912,7 +1960,7 @@
         <v>25</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -1920,10 +1968,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2012,7 +2060,7 @@
         <v>25</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2020,10 +2068,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2112,7 +2160,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2120,10 +2168,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2131,7 +2179,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2140,7 +2188,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2216,7 +2264,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2224,10 +2272,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2235,7 +2283,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2244,7 +2292,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2320,7 +2368,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2328,10 +2376,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2339,7 +2387,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2348,7 +2396,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2424,7 +2472,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2432,10 +2480,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2443,7 +2491,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2452,7 +2500,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2528,7 +2576,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2536,10 +2584,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2547,7 +2595,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2556,7 +2604,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2632,7 +2680,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2640,10 +2688,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2651,7 +2699,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2660,7 +2708,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2754,8 +2802,12 @@
       <c r="E2" s="11"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>29</v>
+      </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -2836,7 +2888,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2844,10 +2896,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2855,7 +2907,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2864,7 +2916,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -2940,7 +2992,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -2948,10 +3000,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -2959,7 +3011,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -2968,7 +3020,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="27">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -3049,7 +3101,7 @@
     </row>
     <row r="2" ht="16.4" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3058,7 +3110,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3147,7 +3199,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3156,7 +3208,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3245,7 +3297,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3254,7 +3306,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3343,7 +3395,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3352,7 +3404,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="27">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3440,7 +3492,7 @@
         <v>25</v>
       </c>
       <c r="C1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="11"/>
@@ -3453,22 +3505,34 @@
         <v>27</v>
       </c>
       <c r="C2" t="s" s="14">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>33</v>
+      </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="A4" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s" s="10">
+        <v>35</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
@@ -3545,10 +3609,10 @@
         <v>25</v>
       </c>
       <c r="C1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E1" s="13"/>
     </row>
@@ -3557,21 +3621,29 @@
         <v>26</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="14">
+        <v>39</v>
+      </c>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="D3" t="s" s="10">
+        <v>42</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
@@ -3654,10 +3726,10 @@
         <v>25</v>
       </c>
       <c r="C1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E1" s="13"/>
     </row>
@@ -3666,21 +3738,29 @@
         <v>26</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="14">
+        <v>39</v>
+      </c>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="D3" t="s" s="10">
+        <v>45</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
@@ -3763,33 +3843,41 @@
         <v>25</v>
       </c>
       <c r="C1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E1" s="13"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="14">
+        <v>39</v>
+      </c>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="D3" t="s" s="10">
+        <v>42</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
@@ -3874,33 +3962,41 @@
         <v>25</v>
       </c>
       <c r="C1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E1" s="13"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s" s="14">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s" s="14">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s" s="14">
+        <v>39</v>
+      </c>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s" s="10">
         <v>35</v>
       </c>
-      <c r="C2" t="s" s="14">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s" s="14">
-        <v>33</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="D3" t="s" s="10">
+        <v>45</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
@@ -3979,7 +4075,7 @@
         <v>25</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -3987,10 +4083,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -4079,7 +4175,7 @@
         <v>25</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="11"/>
@@ -4087,10 +4183,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="14">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>

</xml_diff>

<commit_message>
fix williamchong (Liker Land) phase 1 formatting
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>TeamName</t>
   </si>
@@ -59,30 +59,6 @@
   </si>
   <si>
     <t>Community</t>
-  </si>
-  <si>
-    <t>team name</t>
-  </si>
-  <si>
-    <t>addr1</t>
-  </si>
-  <si>
-    <t>addr2</t>
-  </si>
-  <si>
-    <t>addr3</t>
-  </si>
-  <si>
-    <t>addr4</t>
-  </si>
-  <si>
-    <t>addr5</t>
-  </si>
-  <si>
-    <t>discord#1234</t>
-  </si>
-  <si>
-    <t>set none if no community</t>
   </si>
   <si>
     <t>Liker Land</t>
@@ -115,12 +91,6 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
     <t>F9D6A76D97EE94FA4BFBEB7FB9807E14EE19FFEA5909CA83C22B93970131064B</t>
   </si>
   <si>
@@ -128,9 +98,6 @@
   </si>
   <si>
     <t>NFTID</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
   </si>
   <si>
     <t>73E3720846E6EA59D7B39ADE2122FB2D3CEA698D87E56E7243A06BAB5855BF04</t>
@@ -146,15 +113,6 @@
   </si>
   <si>
     <t>ChainID</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
   </si>
   <si>
     <t>08E95B608EFE04518CCE6FBFD050059BFDE5A99ECE2247C5BF5AC8FC55E48426</t>
@@ -175,16 +133,16 @@
     <t>gon-flixnet-1</t>
   </si>
   <si>
-    <t>tx hash on dest chain</t>
+    <t>AB85B3B1363C71657FB62C2BEDEF814EF5C12DE92C097B959C88ACF2F09D8FD3</t>
+  </si>
+  <si>
+    <t>3179F724E31D62F798F6F314DB6FABF158BD017CC49BDF1695BEFCC1F88BE310</t>
   </si>
   <si>
     <t>ibc class on chain</t>
   </si>
   <si>
-    <t>AB85B3B1363C71657FB62C2BEDEF814EF5C12DE92C097B959C88ACF2F09D8FD3</t>
-  </si>
-  <si>
-    <t>3179F724E31D62F798F6F314DB6FABF158BD017CC49BDF1695BEFCC1F88BE310</t>
+    <t>nft id</t>
   </si>
   <si>
     <t>tx hash on that chain</t>
@@ -256,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -292,31 +250,6 @@
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -351,10 +284,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -369,7 +313,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -385,34 +329,25 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -433,6 +368,9 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -451,7 +389,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1615,123 +1553,107 @@
       <c r="A2" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="E2" t="s" s="7">
+      <c r="E2" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="F2" t="s" s="6">
+      <c r="F2" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="G2" t="s" s="6">
+      <c r="G2" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="H2" t="s" s="8">
+      <c r="H2" t="s" s="6">
         <v>15</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s" s="10">
-        <v>23</v>
-      </c>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -1750,88 +1672,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="22" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="22" customWidth="1"/>
+    <col min="1" max="1" width="16" style="20" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -1850,88 +1772,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="23" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="23" customWidth="1"/>
+    <col min="1" max="1" width="16" style="21" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -1950,88 +1872,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="24" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="24" customWidth="1"/>
+    <col min="1" max="1" width="16" style="22" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2050,88 +1972,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="25" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="25" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="25" customWidth="1"/>
+    <col min="1" max="1" width="16" style="23" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2150,92 +2072,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="26" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="26" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="26" customWidth="1"/>
+    <col min="1" max="1" width="16" style="24" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2254,92 +2176,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="28" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="28" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="28" customWidth="1"/>
+    <col min="1" max="1" width="16" style="26" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="26" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2358,92 +2280,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="29" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="29" customWidth="1"/>
+    <col min="1" max="1" width="16" style="27" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="27" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2462,92 +2384,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="30" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="30" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="30" customWidth="1"/>
+    <col min="1" max="1" width="16" style="28" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="28" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2566,92 +2488,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="31" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="31" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="31" customWidth="1"/>
+    <col min="1" max="1" width="16" style="29" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2670,92 +2592,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="32" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="32" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="32" customWidth="1"/>
+    <col min="1" max="1" width="16" style="30" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2774,92 +2696,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="17.8516" style="12" customWidth="1"/>
-    <col min="3" max="5" width="12.6719" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="12" customWidth="1"/>
+    <col min="1" max="2" width="17.8516" style="8" customWidth="1"/>
+    <col min="3" max="5" width="12.6719" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="A1" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>27</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2878,92 +2796,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="33" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="33" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="33" customWidth="1"/>
+    <col min="1" max="1" width="16" style="31" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -2982,92 +2900,92 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="34" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="34" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="34" customWidth="1"/>
+    <col min="1" max="1" width="16" style="32" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="32" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>51</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="18">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" t="s" s="25">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -3086,85 +3004,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="35" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="35" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="33" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="16.4" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>53</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>39</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>54</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>40</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -3184,85 +3102,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="36" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="36" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>53</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>39</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>54</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>40</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -3282,85 +3200,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="37" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="37" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>53</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>39</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>54</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>40</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -3380,85 +3298,85 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="38" customWidth="1"/>
+    <col min="1" max="5" width="11.5" style="36" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>53</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>39</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>54</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" t="s" s="25">
+        <v>40</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
@@ -3478,105 +3396,99 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="17.8516" style="15" customWidth="1"/>
-    <col min="3" max="3" width="16" style="15" customWidth="1"/>
-    <col min="4" max="5" width="12.6719" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="15" customWidth="1"/>
+    <col min="1" max="2" width="17.8516" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16" style="12" customWidth="1"/>
+    <col min="4" max="5" width="12.6719" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="6">
         <v>24</v>
       </c>
-      <c r="B1" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s" s="14">
-        <v>31</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="10">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s" s="10">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -3595,105 +3507,97 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="17.8516" style="16" customWidth="1"/>
-    <col min="3" max="3" width="16" style="16" customWidth="1"/>
-    <col min="4" max="5" width="12.6719" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="16" customWidth="1"/>
+    <col min="1" max="2" width="17.8516" style="13" customWidth="1"/>
+    <col min="3" max="3" width="16" style="13" customWidth="1"/>
+    <col min="4" max="5" width="12.6719" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s" s="3">
+      <c r="A1" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s" s="10">
         <v>25</v>
       </c>
-      <c r="C1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
+      <c r="A2" t="s" s="6">
         <v>26</v>
       </c>
-      <c r="B2" t="s" s="14">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s" s="14">
-        <v>39</v>
-      </c>
-      <c r="E2" s="11"/>
+      <c r="B2" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s" s="10">
-        <v>42</v>
-      </c>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -3712,105 +3616,97 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="17.8516" style="17" customWidth="1"/>
-    <col min="3" max="3" width="16" style="17" customWidth="1"/>
-    <col min="4" max="5" width="12.6719" style="17" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="17" customWidth="1"/>
+    <col min="1" max="2" width="17.8516" style="14" customWidth="1"/>
+    <col min="3" max="3" width="16" style="14" customWidth="1"/>
+    <col min="4" max="5" width="12.6719" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s" s="3">
+      <c r="A1" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s" s="10">
         <v>25</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s" s="6">
         <v>30</v>
       </c>
-      <c r="D1" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s" s="14">
-        <v>39</v>
-      </c>
-      <c r="E2" s="11"/>
+      <c r="C2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>31</v>
+      </c>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s" s="10">
-        <v>45</v>
-      </c>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -3829,105 +3725,97 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="17.8516" style="18" customWidth="1"/>
-    <col min="3" max="3" width="16" style="18" customWidth="1"/>
-    <col min="4" max="5" width="12.6719" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="18" customWidth="1"/>
+    <col min="1" max="2" width="17.8516" style="15" customWidth="1"/>
+    <col min="3" max="3" width="16" style="15" customWidth="1"/>
+    <col min="4" max="5" width="12.6719" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s" s="3">
+      <c r="A1" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s" s="10">
         <v>25</v>
       </c>
-      <c r="C1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="E1" s="13"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s" s="14">
-        <v>39</v>
-      </c>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="6">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>28</v>
+      </c>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s" s="10">
-        <v>42</v>
-      </c>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -3946,107 +3834,99 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.8516" style="19" customWidth="1"/>
-    <col min="2" max="2" width="16" style="19" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="19" customWidth="1"/>
-    <col min="4" max="4" width="14.3516" style="19" customWidth="1"/>
-    <col min="5" max="5" width="12.6719" style="19" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="19" customWidth="1"/>
+    <col min="1" max="1" width="17.8516" style="16" customWidth="1"/>
+    <col min="2" max="2" width="16" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="16" customWidth="1"/>
+    <col min="4" max="4" width="14.3516" style="16" customWidth="1"/>
+    <col min="5" max="5" width="12.6719" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s" s="6">
         <v>24</v>
       </c>
-      <c r="B1" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s" s="14">
-        <v>39</v>
-      </c>
-      <c r="E2" s="11"/>
+      <c r="D2" t="s" s="6">
+        <v>31</v>
+      </c>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="10">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s" s="10">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s" s="10">
-        <v>45</v>
-      </c>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -4065,88 +3945,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="20" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="20" customWidth="1"/>
+    <col min="1" max="1" width="16" style="17" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>
@@ -4165,88 +4045,88 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="21" customWidth="1"/>
-    <col min="2" max="5" width="12.6719" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="12.6719" style="21" customWidth="1"/>
+    <col min="1" max="1" width="16" style="19" customWidth="1"/>
+    <col min="2" max="5" width="12.6719" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="12.6719" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="14">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s" s="14">
-        <v>38</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="A2" t="s" s="18">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s" s="18">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511811" footer="0.511811"/>

</xml_diff>

<commit_message>
add williamchong (Liker Land) A7-A18,A20 evidence
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>TeamName</t>
   </si>
@@ -139,19 +139,145 @@
     <t>3179F724E31D62F798F6F314DB6FABF158BD017CC49BDF1695BEFCC1F88BE310</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
+    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+  </si>
+  <si>
+    <t>likea7b</t>
+  </si>
+  <si>
+    <t>nft-transfer/channel-0/nft-transfer/channel-41/nft-transfer/channel-3/like</t>
+  </si>
+  <si>
+    <t>likea82</t>
+  </si>
+  <si>
+    <t>nft-transfer/channel-17/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+  </si>
+  <si>
+    <t>likea9b</t>
+  </si>
+  <si>
+    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-44/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+  </si>
+  <si>
+    <t>likea10a</t>
+  </si>
+  <si>
+    <t>nft-transfer/channel-22/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-41/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+  </si>
+  <si>
+    <t>likea11a</t>
+  </si>
+  <si>
+    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-41/nft-transfer/channel-6/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-24/like</t>
+  </si>
+  <si>
+    <t>likea12a</t>
+  </si>
+  <si>
+    <t>3D259B9F4189A59BA2FC568CA8E7D37CC11DDFEC1E11C9134F50529BD6838807</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>67C94B972F07DA807AD2C4F53956281A20EFD8B2358A0C9B51B55173DDB88387</t>
+  </si>
+  <si>
+    <t>0CAC258005C29FC618AC12AE8A996C892CE9928BFA5AB47BF38C1BC7FBAC2856</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>37F79A1BEC3B16251D176AA2A3F39784F4BA6DC285FCC93BE3023394511442F9</t>
+  </si>
+  <si>
+    <t>4AAB93DA7E0D36D4699438BD3B93CA76BE717C1BA7EAEE2090F2F232BD17E4C8</t>
+  </si>
+  <si>
+    <t>FCEA15445DCAAA7876A8DC35DE62A785EDD1421A27A87F7E32DC0B9126540361</t>
+  </si>
+  <si>
+    <t>52D255022DBA919F9080D181D6E29F3AD7E259071A9DF59104ADD58CD9CBA6C4</t>
+  </si>
+  <si>
+    <t>D85980CDDEB1FB5F84BD186735F54C0B7AFEDEC3AF1195C0E31D157EA53DC60F</t>
+  </si>
+  <si>
+    <t>6C00EF2AB01EE9F4B99F5AE6D05002EE4E09CF5FB3D32DA7AE8FBFFB27031846</t>
+  </si>
+  <si>
+    <t>CCB236305742763CD495101051EAE50A164687D5BA95E0943708826EA5B6CC45</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>43C65D95DD1F7FF9EFABA649614E771E2A6C77873E721FB43A8CE10D21AADED4</t>
+  </si>
+  <si>
+    <t>182D4122BE286497CEE1F1FF986EEC35BD584FE2E7D25076C019403583A6A230</t>
+  </si>
+  <si>
+    <t>766FDCE02A3C92CBAF7DD70C07CF8A6CE4C773A0ABB289F941428A30F197D161</t>
+  </si>
+  <si>
+    <t>E986DF9DE17FEEC9334F1C545AEFC019D28B08D67A041C879A1483785808C997</t>
+  </si>
+  <si>
+    <t>E50D40796B3BCD9FBE61A7B0A3CC7EFA0F16EE6D062D912733D02B67161B26BB</t>
+  </si>
+  <si>
+    <t>D34A14416DE549DADF335DBEE4A4CDA4FF457B81122CD7391030B3918402E001</t>
+  </si>
+  <si>
+    <t>65D473156AA8EF2E1FBFD403344634BEFAEB2CD1FCE4941F737B34DB2DC9196D</t>
+  </si>
+  <si>
+    <t>10853DC05830791BB0A123D68FA24AC75F6796F0750B421070FD25E487E2C68D</t>
+  </si>
+  <si>
+    <t>3E601E25981388B5A382F87DDAC041882289122D239B7BC3598F3737DB09238D</t>
+  </si>
+  <si>
+    <t>B642BBBB1C35E9D927B1445ADD9B37DDD468ACC686B7024B4F6FA9A4053FD713</t>
+  </si>
+  <si>
+    <t>1E1C50370544451B2A8341A77A60D519073CEC29D17C015FB1627ABC3B71F2A6</t>
+  </si>
+  <si>
+    <t>E425050C2A86E977DBF6B6ED5F34D5C2708D4DED343C2770181268079365406F</t>
+  </si>
+  <si>
+    <t>6C5B56AE0C99A183A4644DC58F27D8D7F6D348396293DFDA4BDC557EEA81ED71</t>
+  </si>
+  <si>
+    <t>84D8D951155E21F1B1A36A923865678F4D64A4385AA97009F8A5E37B17972C31</t>
+  </si>
+  <si>
+    <t>19890CDB4AEF1C55B53EAD6F860D52B7D326F8D1C7F236EF1ED7C825FEAC3200</t>
+  </si>
+  <si>
+    <t>81E8E15C72F307688B8CAB75413125C56C9F73B51F90946B4A2234650D554DEA</t>
+  </si>
+  <si>
+    <t>D72FC68F5FF112897034457ACDA0BBE10B45A40AFEEA4E5578BE0DA1FCE20D62</t>
+  </si>
+  <si>
+    <t>650C8A5B50C4D47DB5693284566FCD49EC82FD6BEB217A30832E230254084A42</t>
+  </si>
+  <si>
+    <t>DE7CF2FEA565D8B70FE1C673574F5260534BC7E83FD6264D24354CB7BDF6C9C9</t>
+  </si>
+  <si>
+    <t>1478B9D6CEF08C155901178028A2DEDF5115D84B3FEBC2744A4A456972020614</t>
+  </si>
+  <si>
+    <t>7EE7EC1C4607A80571B5DFAFE6196DDE10A102136A8BB5E7A1A8D9588F5A8D75</t>
+  </si>
+  <si>
+    <t>C8484F3F1D917CBEF890B352F814D298EF6052128458C0DFAD92A76BC7E09D54</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -1690,10 +1816,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1778,10 +1904,10 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" t="s" s="10">
         <v>20</v>
       </c>
       <c r="C1" s="11"/>
@@ -1789,11 +1915,11 @@
       <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="18">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s" s="18">
-        <v>35</v>
+      <c r="A2" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>41</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1890,10 +2016,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1978,10 +2104,10 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" t="s" s="10">
         <v>20</v>
       </c>
       <c r="C1" s="11"/>
@@ -1989,11 +2115,11 @@
       <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="18">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s" s="18">
-        <v>35</v>
+      <c r="A2" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>45</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2090,10 +2216,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2101,25 +2227,33 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2194,10 +2328,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2205,25 +2339,33 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>31</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2298,10 +2440,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2309,25 +2451,33 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>58</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>58</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2402,10 +2552,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2413,25 +2563,33 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>58</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>63</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>58</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2506,10 +2664,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2517,25 +2675,33 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>58</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2610,10 +2776,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2621,25 +2787,33 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>31</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>31</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2814,10 +2988,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2825,39 +2999,47 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+      <c r="A4" s="25"/>
+      <c r="B4" t="s" s="6">
+        <v>58</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="B5" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="B6" t="s" s="6">
+        <v>58</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="B7" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -2918,10 +3100,10 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s" s="18">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2929,39 +3111,55 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B3" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>38</v>
-      </c>
-      <c r="B4" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>31</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" t="s" s="6">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s" s="6">
+        <v>28</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" t="s" s="6">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>50</v>
+      </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -3019,7 +3217,7 @@
     </row>
     <row r="2" ht="16.4" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3028,7 +3226,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3117,7 +3315,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3126,7 +3324,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3215,7 +3413,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3224,7 +3422,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3313,7 +3511,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3322,7 +3520,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -4054,7 +4252,7 @@
       <c r="A1" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" t="s" s="10">
         <v>20</v>
       </c>
       <c r="C1" s="11"/>
@@ -4062,11 +4260,11 @@
       <c r="E1" s="7"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="18">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s" s="18">
-        <v>35</v>
+      <c r="A2" t="s" s="5">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>37</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>

</xml_diff>

<commit_message>
add williamchong (Liker Land) A19 evidence
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>TeamName</t>
   </si>
@@ -256,10 +256,22 @@
     <t>84D8D951155E21F1B1A36A923865678F4D64A4385AA97009F8A5E37B17972C31</t>
   </si>
   <si>
-    <t>19890CDB4AEF1C55B53EAD6F860D52B7D326F8D1C7F236EF1ED7C825FEAC3200</t>
-  </si>
-  <si>
-    <t>81E8E15C72F307688B8CAB75413125C56C9F73B51F90946B4A2234650D554DEA</t>
+    <t>A64164EED6ACE25985986BF913DEBF6639AE16EBB5361</t>
+  </si>
+  <si>
+    <t>845F0B04DB633DFE96C9E5F99D993FECB63BF5980BEEB444A147C66286DFCD2B</t>
+  </si>
+  <si>
+    <t>D5ACDA5D38B838EE7E718C0AC0F537D1018BE16D2467B</t>
+  </si>
+  <si>
+    <t>93F5E2C4E22F3B3E1C91313DCE19220B40A29877EA68EEC6AC948076C34D8BA4</t>
+  </si>
+  <si>
+    <t>0A30498C6CFA5A209C0B2F77BAC785E1F4FFA20C97C6E</t>
+  </si>
+  <si>
+    <t>6E49700B0D04992E02FD35E4DE7C2C3745A1592FF1939422F867EDDC0C7D2354</t>
   </si>
   <si>
     <t>D72FC68F5FF112897034457ACDA0BBE10B45A40AFEEA4E5578BE0DA1FCE20D62</t>
@@ -3009,7 +3021,9 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="25"/>
+      <c r="A4" t="s" s="25">
+        <v>75</v>
+      </c>
       <c r="B4" t="s" s="6">
         <v>58</v>
       </c>
@@ -3018,7 +3032,9 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="7"/>
+      <c r="A5" t="s" s="6">
+        <v>76</v>
+      </c>
       <c r="B5" t="s" s="6">
         <v>50</v>
       </c>
@@ -3027,7 +3043,9 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="7"/>
+      <c r="A6" t="s" s="6">
+        <v>77</v>
+      </c>
       <c r="B6" t="s" s="6">
         <v>58</v>
       </c>
@@ -3036,7 +3054,9 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="7"/>
+      <c r="A7" t="s" s="6">
+        <v>78</v>
+      </c>
       <c r="B7" t="s" s="6">
         <v>28</v>
       </c>
@@ -3100,7 +3120,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s" s="18">
         <v>47</v>
@@ -3111,7 +3131,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s" s="6">
         <v>50</v>
@@ -3122,7 +3142,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="25">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s" s="6">
         <v>28</v>
@@ -3133,7 +3153,7 @@
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s" s="6">
         <v>31</v>
@@ -3144,7 +3164,7 @@
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s" s="6">
         <v>28</v>
@@ -3155,7 +3175,7 @@
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s" s="6">
         <v>50</v>
@@ -3217,7 +3237,7 @@
     </row>
     <row r="2" ht="16.4" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3226,7 +3246,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3315,7 +3335,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3324,7 +3344,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3413,7 +3433,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3422,7 +3442,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3511,7 +3531,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3520,7 +3540,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>

</xml_diff>

<commit_message>
add williamchong (Liker Land) B1 evidence
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
   <si>
     <t>TeamName</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>C8484F3F1D917CBEF890B352F814D298EF6052128458C0DFAD92A76BC7E09D54</t>
+  </si>
+  <si>
+    <t>82197AA3089F868297FF2BA72A0824539241CC17DEF76032DA63C9D859546630</t>
+  </si>
+  <si>
+    <t>013959228966C8429E22F02AB112B690E342AE691A30AC5F443E97FF1066678A</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -3335,7 +3341,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3344,7 +3350,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3433,7 +3439,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3442,7 +3448,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3531,7 +3537,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3540,7 +3546,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>

</xml_diff>

<commit_message>
add williamchong (Liker Land) B2 evidence
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>TeamName</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>013959228966C8429E22F02AB112B690E342AE691A30AC5F443E97FF1066678A</t>
+  </si>
+  <si>
+    <t>C7C96E000C91E97E462CA7503D200964721777E7FA31A918A80A4403F02B4F0C</t>
+  </si>
+  <si>
+    <t>0B7EB16ED9A82FA683DD35B51055DA306E31BEC4C3570609BC83D4E116979503</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
@@ -3439,7 +3445,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3448,7 +3454,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3537,7 +3543,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3546,7 +3552,7 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>

</xml_diff>

<commit_message>
fix williamchong (Liker Land) A7-A12,A19 evidence
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -139,37 +139,37 @@
     <t>3179F724E31D62F798F6F314DB6FABF158BD017CC49BDF1695BEFCC1F88BE310</t>
   </si>
   <si>
-    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+    <t>ibc/EEBF797CF7F3FFD685F8BD3CB88BA477926B4FAC9FF5E083FAAF6953D33F8C8E</t>
   </si>
   <si>
     <t>likea7b</t>
   </si>
   <si>
-    <t>nft-transfer/channel-0/nft-transfer/channel-41/nft-transfer/channel-3/like</t>
+    <t>ibc/DA71C628600F1AD7B8AD47B7564E486C6D88C1DE75D89DB3C60F24DE155CE796</t>
   </si>
   <si>
     <t>likea82</t>
   </si>
   <si>
-    <t>nft-transfer/channel-17/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+    <t>ibc/41DF42E29B453B3F33179589366D0AF7187A6AEA73F7D3909DE088548E07E6C7</t>
   </si>
   <si>
     <t>likea9b</t>
   </si>
   <si>
-    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-44/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+    <t>ibc/A0F76F679A097CA81C9D2B160E069E94F9A8EFF6DA357F6354423CFFBDB88E02</t>
   </si>
   <si>
     <t>likea10a</t>
   </si>
   <si>
-    <t>nft-transfer/channel-22/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-41/nft-transfer/channel-7/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-93/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/like</t>
+    <t>ibc/BBE3FBCB1C8F9E3FB0B48FF4C3971A19DC670C816E5DF21B6F22C039FF45C8C4</t>
   </si>
   <si>
     <t>likea11a</t>
   </si>
   <si>
-    <t>nft-transfer/channel-24/wasm.juno1stv6sk0mvku34fj2mqrlyru6683866n306mfv52tlugtl322zmks26kg7a/channel-91/nft-transfer/channel-41/nft-transfer/channel-6/wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-209/nft-transfer/channel-24/like</t>
+    <t>ibc/88B33E0AF9CED4271FB0D66626C056481D3D65910CDCDEA63AD799DE905B7DE0</t>
   </si>
   <si>
     <t>likea12a</t>
@@ -256,22 +256,22 @@
     <t>84D8D951155E21F1B1A36A923865678F4D64A4385AA97009F8A5E37B17972C31</t>
   </si>
   <si>
-    <t>A64164EED6ACE25985986BF913DEBF6639AE16EBB5361</t>
-  </si>
-  <si>
-    <t>845F0B04DB633DFE96C9E5F99D993FECB63BF5980BEEB444A147C66286DFCD2B</t>
-  </si>
-  <si>
-    <t>D5ACDA5D38B838EE7E718C0AC0F537D1018BE16D2467B</t>
-  </si>
-  <si>
-    <t>93F5E2C4E22F3B3E1C91313DCE19220B40A29877EA68EEC6AC948076C34D8BA4</t>
-  </si>
-  <si>
-    <t>0A30498C6CFA5A209C0B2F77BAC785E1F4FFA20C97C6E</t>
-  </si>
-  <si>
-    <t>6E49700B0D04992E02FD35E4DE7C2C3745A1592FF1939422F867EDDC0C7D2354</t>
+    <t>59E8799336FD4D3D224CE9BC7311BD2749A5881EBD328CB825D1C6952B9E9889</t>
+  </si>
+  <si>
+    <t>2CECA6704D25DC14CB9B5C4C343CA53B4E093EAFDA540BED69381D95B0F68C77</t>
+  </si>
+  <si>
+    <t>8CC26555FF42A35662EA9F88CA9ECCCC0B5C3948A0DEE1E37DD8E1088FE91A20</t>
+  </si>
+  <si>
+    <t>27CB320D276F09B3AEDD2A70F4A028D87012ECDB149F7972813DF7E7D53298BD</t>
+  </si>
+  <si>
+    <t>F2E7810DD54621896ADD4C4D20F57861D69C539463014074C09F5BDF36CE75DC</t>
+  </si>
+  <si>
+    <t>4CBD631DAC38A298651C8671B1CA98006D3320868DC0AAF75B5D40FBB9A9D46C</t>
   </si>
   <si>
     <t>D72FC68F5FF112897034457ACDA0BBE10B45A40AFEEA4E5578BE0DA1FCE20D62</t>

</xml_diff>

<commit_message>
add williamchong (Liker Land) B5-7 evidence
</commit_message>
<xml_diff>
--- a/williamchong/evidence.xlsx
+++ b/williamchong/evidence.xlsx
@@ -30,12 +30,13 @@
     <sheet name="B2" sheetId="23" r:id="rId26"/>
     <sheet name="B5" sheetId="24" r:id="rId27"/>
     <sheet name="B6" sheetId="25" r:id="rId28"/>
+    <sheet name="B7" sheetId="26" r:id="rId29"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>TeamName</t>
   </si>
@@ -304,10 +305,22 @@
     <t>0B7EB16ED9A82FA683DD35B51055DA306E31BEC4C3570609BC83D4E116979503</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
+    <t>8348CE2842BEE3B48D50381FF2462D6F23BD809C5394C73A036725D4887EF902</t>
+  </si>
+  <si>
+    <t>416E2600CF3FCD19AB8A0DF19A801B568A4793B135CF3408018726DA61F31303</t>
+  </si>
+  <si>
+    <t>8BE17FC55ABD5004492374CE4B62E02C51ACFD6843DF80D2B348F41BA3014187</t>
+  </si>
+  <si>
+    <t>08B8C325361A82B662AF973E546F0D38CCCAFE91DA446AC08BF0E4761034F267</t>
+  </si>
+  <si>
+    <t>EF953B9D4B6A076B32B4092F4CCC74060AE25BCC16CFA333D8EB4DB28E6ADBD4</t>
+  </si>
+  <si>
+    <t>BD5368BEF5C29E152889A8888710055D7F4E90922B36506B49CB484C8B95A3A4</t>
   </si>
 </sst>
 </file>
@@ -463,7 +476,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -540,6 +553,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -3543,7 +3559,7 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="18">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3552,7 +3568,105 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="25">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KFFFFFFB6</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KFFFFFFPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13.1" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="11.5" style="37" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s" s="18">
+        <v>93</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" t="s" s="25">
+        <v>94</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>

</xml_diff>